<commit_message>
Update source data to use 'Box' container type
In production ArchivesSpace, 'box' (lowercase) is not a valid
value in the controlled vocabulary for container type, so we need
to use 'Box' (capitalized) instead in order for the data to upload.

This commit applies the change at the item level and then regenerates
the relevant uploader sheets.
</commit_message>
<xml_diff>
--- a/source_data/uploaders/Document books_hierarchy_aspace.xlsx
+++ b/source_data/uploaders/Document books_hierarchy_aspace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbudak/Projects/nta-arclight/source_data/uploaders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6853C149-4757-8248-8B07-EF7B7788EB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255398EC-1632-774E-9898-7347CDC50BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1699,7 +1699,7 @@
     <t>text</t>
   </si>
   <si>
-    <t>box</t>
+    <t>Box</t>
   </si>
   <si>
     <t>6</t>
@@ -7078,7 +7078,7 @@
   <dimension ref="A1:HE399"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add H-2785 and regenerate all data
</commit_message>
<xml_diff>
--- a/source_data/uploaders/Document books_hierarchy_aspace.xlsx
+++ b/source_data/uploaders/Document books_hierarchy_aspace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbudak/Projects/nta-arclight/source_data/uploaders/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marloelilongley/Projects/vt-arclight/source_data/uploaders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255398EC-1632-774E-9898-7347CDC50BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD95A773-7D9E-F847-9B6A-F9DE9E76380C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3040" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>

</xml_diff>